<commit_message>
& - №71036340 от 22.09.2024 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/Russia/#Russia#Russian_Federation#Commemorative#[1999-present]#circulation_quality.xlsx
+++ b/Collections/Russia/#Russia#Russian_Federation#Commemorative#[1999-present]#circulation_quality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\Russia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3C1388-EC06-4B18-B79F-68D4AAF9E18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D169F3-6D8B-4FF8-BE03-119550512CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="1450" windowWidth="28720" windowHeight="19550" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5660" yWindow="1450" windowWidth="28720" windowHeight="19550" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1₽ " sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="381">
   <si>
     <t>-</t>
   </si>
@@ -1556,7 +1556,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1677,6 +1677,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1825,7 +1832,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2013,13 +2020,32 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="174">
+  <dxfs count="176">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3427,9 +3453,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="3" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -4469,7 +4495,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:H3">
-    <cfRule type="containsText" dxfId="173" priority="21" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="175" priority="21" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4486,7 +4512,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="172" priority="19" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="174" priority="19" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G5))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4503,7 +4529,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="171" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="173" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H5))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4520,7 +4546,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="containsText" dxfId="170" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="172" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G4))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4537,7 +4563,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="169" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="171" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4554,7 +4580,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:H18">
-    <cfRule type="containsText" dxfId="168" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="170" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G18))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4571,7 +4597,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G17">
-    <cfRule type="containsText" dxfId="167" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="169" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G6))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4588,7 +4614,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H17">
-    <cfRule type="containsText" dxfId="166" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="168" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H6))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4605,7 +4631,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G28">
-    <cfRule type="containsText" dxfId="165" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="167" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G19))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4622,7 +4648,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H28">
-    <cfRule type="containsText" dxfId="164" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="166" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H19))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5734,7 +5760,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:H31">
-    <cfRule type="containsText" dxfId="163" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="165" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G4))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -5749,7 +5775,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="containsText" dxfId="162" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="164" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -5764,7 +5790,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="161" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="163" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -5779,7 +5805,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G38">
-    <cfRule type="containsText" dxfId="160" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="162" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G32))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -5794,7 +5820,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H38">
-    <cfRule type="containsText" dxfId="159" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="161" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H32))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -7847,7 +7873,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G16:H65 G3:H8">
-    <cfRule type="containsText" dxfId="158" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="160" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="18">
@@ -7862,7 +7888,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66">
-    <cfRule type="containsText" dxfId="157" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="159" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H66))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -7877,7 +7903,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G15">
-    <cfRule type="containsText" dxfId="156" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="158" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G9))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -7892,7 +7918,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H15">
-    <cfRule type="containsText" dxfId="155" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="157" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H9))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="12">
@@ -7907,7 +7933,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G67:G71">
-    <cfRule type="containsText" dxfId="154" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="156" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G67))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -7922,7 +7948,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67:H71">
-    <cfRule type="containsText" dxfId="153" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="155" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H67))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -7937,7 +7963,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="containsText" dxfId="152" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="154" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G66))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7963,11 +7989,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J162" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="9" ySplit="2" topLeftCell="J24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J191" sqref="J191"/>
+      <selection pane="bottomRight" activeCell="A123" sqref="A123:XFD123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -9388,10 +9414,10 @@
         <v>176</v>
       </c>
       <c r="G48" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" s="33" t="str">
         <f t="shared" si="2"/>
@@ -9418,7 +9444,7 @@
         <v>176</v>
       </c>
       <c r="G49" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" s="13">
         <v>1</v>
@@ -9451,7 +9477,7 @@
         <v>2</v>
       </c>
       <c r="H50" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="33" t="str">
         <f t="shared" si="2"/>
@@ -9478,7 +9504,7 @@
         <v>176</v>
       </c>
       <c r="G51" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="11">
         <v>1</v>
@@ -9511,7 +9537,7 @@
         <v>1</v>
       </c>
       <c r="H52" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="33" t="str">
         <f t="shared" si="2"/>
@@ -9538,7 +9564,7 @@
         <v>176</v>
       </c>
       <c r="G53" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" s="13">
         <v>1</v>
@@ -9691,7 +9717,7 @@
         <v>1</v>
       </c>
       <c r="H58" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" s="33" t="str">
         <f t="shared" si="2"/>
@@ -9781,7 +9807,7 @@
         <v>1</v>
       </c>
       <c r="H61" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" s="33" t="str">
         <f t="shared" si="2"/>
@@ -13859,7 +13885,7 @@
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="G4:H108 G109 G110:H167">
-    <cfRule type="containsText" dxfId="151" priority="65" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="153" priority="65" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G4))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="66">
@@ -13874,7 +13900,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G168:H168">
-    <cfRule type="containsText" dxfId="150" priority="63" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="152" priority="63" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G168))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="64">
@@ -13889,7 +13915,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G169:H169">
-    <cfRule type="containsText" dxfId="149" priority="61" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="151" priority="61" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G169))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="62">
@@ -13904,7 +13930,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G170:H170">
-    <cfRule type="containsText" dxfId="148" priority="59" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="150" priority="59" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G170))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="60">
@@ -13919,7 +13945,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G171:H171">
-    <cfRule type="containsText" dxfId="147" priority="57" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="149" priority="57" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G171))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="58">
@@ -13934,7 +13960,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G172:H172">
-    <cfRule type="containsText" dxfId="146" priority="55" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="148" priority="55" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G172))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="56">
@@ -13949,7 +13975,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G173:H173">
-    <cfRule type="containsText" dxfId="145" priority="53" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="147" priority="53" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G173))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="54">
@@ -13964,7 +13990,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G174:H174">
-    <cfRule type="containsText" dxfId="144" priority="51" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="146" priority="51" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G174))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="52">
@@ -13979,7 +14005,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G175:H175">
-    <cfRule type="containsText" dxfId="143" priority="49" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="145" priority="49" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G175))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="50">
@@ -13994,7 +14020,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G176:H176">
-    <cfRule type="containsText" dxfId="142" priority="47" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="144" priority="47" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G176))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="48">
@@ -14009,7 +14035,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G177:H177">
-    <cfRule type="containsText" dxfId="141" priority="45" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="143" priority="45" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G177))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="46">
@@ -14024,7 +14050,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G178:H178">
-    <cfRule type="containsText" dxfId="140" priority="43" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="142" priority="43" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G178))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="44">
@@ -14039,7 +14065,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G179:H179">
-    <cfRule type="containsText" dxfId="139" priority="41" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="141" priority="41" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G179))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="42">
@@ -14054,7 +14080,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G180:H180">
-    <cfRule type="containsText" dxfId="138" priority="39" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="140" priority="39" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G180))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="40">
@@ -14069,7 +14095,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:H181">
-    <cfRule type="containsText" dxfId="137" priority="37" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="139" priority="37" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G181))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="38">
@@ -14084,7 +14110,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:H182">
-    <cfRule type="containsText" dxfId="136" priority="33" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="138" priority="33" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G182))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="34">
@@ -14099,7 +14125,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:H183">
-    <cfRule type="containsText" dxfId="135" priority="31" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="137" priority="31" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G183))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="32">
@@ -14114,7 +14140,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:H184">
-    <cfRule type="containsText" dxfId="134" priority="29" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="136" priority="29" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G184))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="30">
@@ -14129,7 +14155,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186:H186">
-    <cfRule type="containsText" dxfId="133" priority="25" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="135" priority="25" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G186))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="26">
@@ -14144,7 +14170,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:H187">
-    <cfRule type="containsText" dxfId="132" priority="23" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="134" priority="23" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G187))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="24">
@@ -14159,7 +14185,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188:H188">
-    <cfRule type="containsText" dxfId="131" priority="21" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="133" priority="21" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G188))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="22">
@@ -14174,7 +14200,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="containsText" dxfId="130" priority="19" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="132" priority="19" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G185))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="20">
@@ -14189,7 +14215,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:H189">
-    <cfRule type="containsText" dxfId="129" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="131" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G189))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="18">
@@ -14204,7 +14230,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190:H190">
-    <cfRule type="containsText" dxfId="128" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="130" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G190))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -14219,7 +14245,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:H191">
-    <cfRule type="containsText" dxfId="127" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="129" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G191))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -14234,7 +14260,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109">
-    <cfRule type="containsText" dxfId="126" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="128" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H109))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14251,7 +14277,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:H3">
-    <cfRule type="containsText" dxfId="125" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="127" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -14266,7 +14292,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G192">
-    <cfRule type="containsText" dxfId="124" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="126" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G192))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -14281,7 +14307,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H192">
-    <cfRule type="containsText" dxfId="123" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="125" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H192))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -14296,7 +14322,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G193:H193 G195:H195 G197:H197">
-    <cfRule type="containsText" dxfId="122" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="124" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G193))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -14311,7 +14337,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G194:H194 G196:H196">
-    <cfRule type="containsText" dxfId="121" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="123" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G194))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -14335,11 +14361,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J54" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="9" ySplit="2" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -15194,8 +15220,8 @@
       <c r="F30" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>0</v>
+      <c r="G30" s="67">
+        <v>1</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>0</v>
@@ -15276,7 +15302,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>0</v>
@@ -16855,7 +16881,7 @@
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="G15:H15 G17:H17 G26:H26 G19:H20 G22:H24">
-    <cfRule type="containsText" dxfId="120" priority="366" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="122" priority="366" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G15))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="367">
@@ -16870,7 +16896,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="containsText" dxfId="119" priority="347" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="121" priority="347" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H26))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16887,7 +16913,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:H28">
-    <cfRule type="containsText" dxfId="118" priority="345" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="120" priority="345" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G28))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="346">
@@ -16902,7 +16928,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="containsText" dxfId="117" priority="343" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="119" priority="343" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H28))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16919,7 +16945,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:H30">
-    <cfRule type="containsText" dxfId="116" priority="341" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="118" priority="341" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G30))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="342">
@@ -16934,7 +16960,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsText" dxfId="115" priority="339" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="117" priority="339" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H30))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16951,7 +16977,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:H32">
-    <cfRule type="containsText" dxfId="114" priority="333" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="116" priority="333" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G32))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="334">
@@ -16966,7 +16992,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="113" priority="331" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="115" priority="331" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H32))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16983,7 +17009,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:H34 G38:H38">
-    <cfRule type="containsText" dxfId="112" priority="329" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="114" priority="329" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G34))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="330">
@@ -16998,11 +17024,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34 H38">
-    <cfRule type="containsText" dxfId="111" priority="327" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="113" priority="327" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H34))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34 H38">
+  <conditionalFormatting sqref="H38 H34">
     <cfRule type="colorScale" priority="328">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17015,7 +17041,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:H33 G36:H36 G40:H40">
-    <cfRule type="containsText" dxfId="110" priority="325" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="112" priority="325" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G33))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="326">
@@ -17030,11 +17056,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33 H36 H40">
-    <cfRule type="containsText" dxfId="109" priority="323" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="111" priority="323" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H33))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33 H36 H40">
+  <conditionalFormatting sqref="H36 H33 H40">
     <cfRule type="colorScale" priority="324">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17047,7 +17073,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:H42">
-    <cfRule type="containsText" dxfId="108" priority="321" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="110" priority="321" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G42))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="322">
@@ -17062,7 +17088,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="containsText" dxfId="107" priority="319" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="109" priority="319" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H42))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17079,7 +17105,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:H43">
-    <cfRule type="containsText" dxfId="106" priority="317" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="108" priority="317" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G43))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="318">
@@ -17094,7 +17120,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="containsText" dxfId="105" priority="315" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="107" priority="315" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H43))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17111,7 +17137,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:H45">
-    <cfRule type="containsText" dxfId="104" priority="313" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="106" priority="313" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G45))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="314">
@@ -17126,7 +17152,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="containsText" dxfId="103" priority="311" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="105" priority="311" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H45))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17143,7 +17169,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47:H47 G49:H49 G51:H51 G53:H53 G55:H56 G54">
-    <cfRule type="containsText" dxfId="102" priority="309" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="104" priority="309" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G47))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="310">
@@ -17158,11 +17184,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47 H49 H51 H53 H55:H56">
-    <cfRule type="containsText" dxfId="101" priority="307" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="103" priority="307" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H47))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47 H49 H51 H53 H55:H56">
+  <conditionalFormatting sqref="H49 H47 H51 H53 H55:H56">
     <cfRule type="colorScale" priority="308">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17175,7 +17201,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48:H48 G50:H50 G52:H52 H54">
-    <cfRule type="containsText" dxfId="100" priority="305" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="102" priority="305" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G48))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="306">
@@ -17190,11 +17216,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48 H50 H52 H54">
-    <cfRule type="containsText" dxfId="99" priority="303" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="101" priority="303" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H48))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48 H50 H52 H54">
+  <conditionalFormatting sqref="H50 H48 H52 H54">
     <cfRule type="colorScale" priority="304">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17207,7 +17233,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G61:H61 G63:H63 G65:H65 G67:H67 G69:H69">
-    <cfRule type="containsText" dxfId="98" priority="281" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="100" priority="281" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G61))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="282">
@@ -17222,11 +17248,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61 H63 H65 H67 H69">
-    <cfRule type="containsText" dxfId="97" priority="279" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="99" priority="279" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H61))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H61 H63 H65 H67 H69">
+  <conditionalFormatting sqref="H63 H61 H65 H67 H69">
     <cfRule type="colorScale" priority="280">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17239,7 +17265,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:H60 G62:H62 G64:H64 G66:H66 G68:H68 G70:H70 G73:H73">
-    <cfRule type="containsText" dxfId="96" priority="277" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="98" priority="277" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G60))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="278">
@@ -17254,11 +17280,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60 H62 H64 H66 H68 H70 H73">
-    <cfRule type="containsText" dxfId="95" priority="275" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="97" priority="275" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H60))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H60 H62 H64 H66 H68 H70 H73">
+  <conditionalFormatting sqref="H62 H60 H64 H66 H68 H70 H73">
     <cfRule type="colorScale" priority="276">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17271,7 +17297,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58:H58">
-    <cfRule type="containsText" dxfId="94" priority="273" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="96" priority="273" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G58))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="274">
@@ -17286,7 +17312,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="containsText" dxfId="93" priority="271" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="95" priority="271" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H58))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17303,7 +17329,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G71:H71">
-    <cfRule type="containsText" dxfId="92" priority="269" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="94" priority="269" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G71))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="270">
@@ -17318,7 +17344,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71">
-    <cfRule type="containsText" dxfId="91" priority="267" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="93" priority="267" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H71))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17335,7 +17361,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="containsText" dxfId="90" priority="253" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="92" priority="253" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G22))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="254">
@@ -17350,7 +17376,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="89" priority="251" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="91" priority="251" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H22))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="252">
@@ -17365,7 +17391,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="containsText" dxfId="88" priority="249" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="90" priority="249" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G25))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="250">
@@ -17380,7 +17406,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27:H27">
-    <cfRule type="containsText" dxfId="87" priority="241" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="89" priority="241" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G27))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="242">
@@ -17395,7 +17421,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="86" priority="239" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="88" priority="239" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H27))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17412,7 +17438,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G75:H75">
-    <cfRule type="containsText" dxfId="85" priority="189" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="87" priority="189" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G75))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="190">
@@ -17427,7 +17453,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="containsText" dxfId="84" priority="187" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="86" priority="187" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H75))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17444,7 +17470,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G77:H77">
-    <cfRule type="containsText" dxfId="83" priority="181" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="85" priority="181" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G77))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="182">
@@ -17459,7 +17485,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="containsText" dxfId="82" priority="179" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="84" priority="179" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H77))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17476,7 +17502,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:H79">
-    <cfRule type="containsText" dxfId="81" priority="173" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="83" priority="173" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G79))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="174">
@@ -17491,7 +17517,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="containsText" dxfId="80" priority="171" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="82" priority="171" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H79))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17508,7 +17534,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81:H81">
-    <cfRule type="containsText" dxfId="79" priority="169" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="81" priority="169" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G81))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="170">
@@ -17523,7 +17549,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81">
-    <cfRule type="containsText" dxfId="78" priority="167" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="80" priority="167" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H81))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17540,7 +17566,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83:H83">
-    <cfRule type="containsText" dxfId="77" priority="165" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="79" priority="165" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G83))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="166">
@@ -17555,7 +17581,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="containsText" dxfId="76" priority="163" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="78" priority="163" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H83))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17572,7 +17598,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G85:H85">
-    <cfRule type="containsText" dxfId="75" priority="161" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="77" priority="161" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G85))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="162">
@@ -17587,7 +17613,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="containsText" dxfId="74" priority="159" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="76" priority="159" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H85))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17604,7 +17630,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="containsText" dxfId="73" priority="141" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="75" priority="141" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G27))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17621,7 +17647,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:H29">
-    <cfRule type="containsText" dxfId="72" priority="139" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="74" priority="139" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G29))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="140">
@@ -17636,7 +17662,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="containsText" dxfId="71" priority="137" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="73" priority="137" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H29))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17653,7 +17679,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="containsText" dxfId="70" priority="135" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="72" priority="135" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G29))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17670,7 +17696,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35:H35">
-    <cfRule type="containsText" dxfId="69" priority="133" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="71" priority="133" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G35))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="134">
@@ -17685,7 +17711,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="containsText" dxfId="68" priority="131" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="70" priority="131" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H35))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17702,7 +17728,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="67" priority="129" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="69" priority="129" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G35))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17719,7 +17745,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44:H44">
-    <cfRule type="containsText" dxfId="66" priority="127" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="68" priority="127" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G44))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="128">
@@ -17734,7 +17760,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="containsText" dxfId="65" priority="125" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="67" priority="125" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H44))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17751,7 +17777,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44">
-    <cfRule type="containsText" dxfId="64" priority="123" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="66" priority="123" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G44))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17768,7 +17794,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46:H46">
-    <cfRule type="containsText" dxfId="63" priority="121" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="65" priority="121" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G46))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="122">
@@ -17783,7 +17809,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="containsText" dxfId="62" priority="119" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="64" priority="119" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H46))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17800,7 +17826,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46">
-    <cfRule type="containsText" dxfId="61" priority="117" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="63" priority="117" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G46))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17817,7 +17843,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G59:H59">
-    <cfRule type="containsText" dxfId="60" priority="115" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="62" priority="115" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G59))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="116">
@@ -17832,7 +17858,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="containsText" dxfId="59" priority="113" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="61" priority="113" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H59))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17849,7 +17875,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G59">
-    <cfRule type="containsText" dxfId="58" priority="111" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="60" priority="111" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G59))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17866,7 +17892,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:H57">
-    <cfRule type="containsText" dxfId="57" priority="109" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="59" priority="109" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G57))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="110">
@@ -17881,7 +17907,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="containsText" dxfId="56" priority="107" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="58" priority="107" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H57))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17898,7 +17924,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="containsText" dxfId="55" priority="105" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="57" priority="105" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G57))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17915,7 +17941,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G80:H80">
-    <cfRule type="containsText" dxfId="54" priority="103" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="56" priority="103" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G80))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="104">
@@ -17930,7 +17956,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="containsText" dxfId="53" priority="101" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="55" priority="101" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H80))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17947,7 +17973,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G80">
-    <cfRule type="containsText" dxfId="52" priority="99" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="54" priority="99" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G80))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17964,7 +17990,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G78:H78">
-    <cfRule type="containsText" dxfId="51" priority="97" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="53" priority="97" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G78))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="98">
@@ -17979,7 +18005,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78">
-    <cfRule type="containsText" dxfId="50" priority="95" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="52" priority="95" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H78))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17996,7 +18022,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G78">
-    <cfRule type="containsText" dxfId="49" priority="93" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="51" priority="93" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G78))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18013,7 +18039,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76:H76">
-    <cfRule type="containsText" dxfId="48" priority="91" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="50" priority="91" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G76))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="92">
@@ -18028,7 +18054,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76">
-    <cfRule type="containsText" dxfId="47" priority="89" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="49" priority="89" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H76))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18045,7 +18071,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76">
-    <cfRule type="containsText" dxfId="46" priority="87" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="48" priority="87" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G76))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18062,7 +18088,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G74:H74">
-    <cfRule type="containsText" dxfId="45" priority="85" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="47" priority="85" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G74))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="86">
@@ -18077,7 +18103,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74">
-    <cfRule type="containsText" dxfId="44" priority="83" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="46" priority="83" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H74))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18094,7 +18120,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G74">
-    <cfRule type="containsText" dxfId="43" priority="81" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="45" priority="81" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G74))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18111,7 +18137,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G72:H72">
-    <cfRule type="containsText" dxfId="42" priority="79" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="44" priority="79" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G72))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="80">
@@ -18126,7 +18152,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72">
-    <cfRule type="containsText" dxfId="41" priority="77" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="43" priority="77" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H72))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18143,7 +18169,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G72">
-    <cfRule type="containsText" dxfId="40" priority="75" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="42" priority="75" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G72))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18160,7 +18186,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82:H82">
-    <cfRule type="containsText" dxfId="39" priority="73" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="41" priority="73" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G82))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="74">
@@ -18175,7 +18201,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="containsText" dxfId="38" priority="71" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="40" priority="71" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H82))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18192,7 +18218,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82">
-    <cfRule type="containsText" dxfId="37" priority="69" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="39" priority="69" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G82))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18209,7 +18235,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86:H86">
-    <cfRule type="containsText" dxfId="36" priority="67" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="38" priority="67" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G86))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="68">
@@ -18224,7 +18250,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="containsText" dxfId="35" priority="65" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="37" priority="65" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H86))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18241,7 +18267,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86">
-    <cfRule type="containsText" dxfId="34" priority="63" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="36" priority="63" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G86))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18258,7 +18284,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G84:H84">
-    <cfRule type="containsText" dxfId="33" priority="61" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="35" priority="61" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G84))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="62">
@@ -18273,7 +18299,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="containsText" dxfId="32" priority="59" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="34" priority="59" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H84))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18290,7 +18316,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G84">
-    <cfRule type="containsText" dxfId="31" priority="57" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="33" priority="57" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G84))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18307,7 +18333,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:H37">
-    <cfRule type="containsText" dxfId="30" priority="55" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="32" priority="55" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G37))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="56">
@@ -18322,7 +18348,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="containsText" dxfId="29" priority="53" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="31" priority="53" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H37))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18339,7 +18365,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="containsText" dxfId="28" priority="51" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="30" priority="51" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G37))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18356,7 +18382,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41:H41">
-    <cfRule type="containsText" dxfId="27" priority="49" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="29" priority="49" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G41))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="50">
@@ -18371,7 +18397,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="containsText" dxfId="26" priority="47" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="28" priority="47" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H41))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18388,7 +18414,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41">
-    <cfRule type="containsText" dxfId="25" priority="45" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="27" priority="45" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G41))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18405,7 +18431,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39:H39">
-    <cfRule type="containsText" dxfId="24" priority="43" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="26" priority="43" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G39))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="44">
@@ -18420,7 +18446,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="containsText" dxfId="23" priority="41" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="25" priority="41" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H39))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18437,7 +18463,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="containsText" dxfId="22" priority="39" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="24" priority="39" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G39))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18454,7 +18480,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="containsText" dxfId="21" priority="37" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="23" priority="37" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H25))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="38">
@@ -18469,7 +18495,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="containsText" dxfId="20" priority="35" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="22" priority="35" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G21))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="36">
@@ -18484,7 +18510,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="19" priority="33" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="21" priority="33" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H21))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="34">
@@ -18499,7 +18525,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="containsText" dxfId="18" priority="31" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G18))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="32">
@@ -18514,7 +18540,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="17" priority="29" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H18))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="30">
@@ -18529,7 +18555,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="containsText" dxfId="16" priority="27" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="18" priority="27" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G16))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="28">
@@ -18544,7 +18570,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="26">
@@ -18559,7 +18585,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G30))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18576,7 +18602,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:H31">
-    <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G31))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="22">
@@ -18591,7 +18617,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="containsText" dxfId="12" priority="19" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H31))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18608,7 +18634,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G31))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18625,7 +18651,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:H8">
-    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -18640,7 +18666,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G14">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G9))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -18655,7 +18681,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H14">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H9))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="12">
@@ -18670,7 +18696,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G87:H87">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G87))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -18685,7 +18711,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H87))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18702,7 +18728,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88:H88">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G88))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -18717,7 +18743,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H88))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18734,7 +18760,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G88))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
& # - Актуализация - №71039102 от 22.09.2024 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/Russia/#Russia#Russian_Federation#Commemorative#[1999-present]#circulation_quality.xlsx
+++ b/Collections/Russia/#Russia#Russian_Federation#Commemorative#[1999-present]#circulation_quality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\Russia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D169F3-6D8B-4FF8-BE03-119550512CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005D0B53-FD70-4038-B5D6-155A29700866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="1450" windowWidth="28720" windowHeight="19550" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4910" yWindow="630" windowWidth="28720" windowHeight="19550" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1₽ " sheetId="1" r:id="rId1"/>
@@ -1982,6 +1982,9 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2020,32 +2023,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="176">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BE5FF"/>
-          <bgColor rgb="FF9BE5FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BE5FF"/>
-          <bgColor rgb="FF9BE5FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="174">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3453,9 +3437,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="3" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -3744,29 +3728,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="55" t="s">
+      <c r="A1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>341</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="57" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="59" t="s">
+      <c r="F1" s="59"/>
+      <c r="G1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="60"/>
+      <c r="H1" s="61"/>
       <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -4495,7 +4479,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:H3">
-    <cfRule type="containsText" dxfId="175" priority="21" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="173" priority="21" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4512,7 +4496,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="containsText" dxfId="174" priority="19" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="172" priority="19" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G5))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4529,7 +4513,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="containsText" dxfId="173" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="171" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H5))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4546,7 +4530,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="containsText" dxfId="172" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="170" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G4))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4563,7 +4547,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="containsText" dxfId="171" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="169" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4580,7 +4564,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:H18">
-    <cfRule type="containsText" dxfId="170" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="168" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G18))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4597,7 +4581,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G17">
-    <cfRule type="containsText" dxfId="169" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="167" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G6))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4614,7 +4598,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H17">
-    <cfRule type="containsText" dxfId="168" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="166" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H6))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4631,7 +4615,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:G28">
-    <cfRule type="containsText" dxfId="167" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="165" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G19))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4648,7 +4632,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H28">
-    <cfRule type="containsText" dxfId="166" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="164" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H19))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4693,29 +4677,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="55" t="s">
+      <c r="A1" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>341</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="62" t="s">
+      <c r="D1" s="64"/>
+      <c r="E1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="65"/>
+      <c r="H1" s="66"/>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="27" t="s">
         <v>4</v>
       </c>
@@ -5760,7 +5744,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:H31">
-    <cfRule type="containsText" dxfId="165" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="163" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G4))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -5775,7 +5759,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="containsText" dxfId="164" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="162" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -5790,7 +5774,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="163" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="161" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -5805,7 +5789,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:G38">
-    <cfRule type="containsText" dxfId="162" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="160" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G32))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -5820,7 +5804,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H38">
-    <cfRule type="containsText" dxfId="161" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="159" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H32))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -5863,29 +5847,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="55" t="s">
+      <c r="A1" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>341</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="62" t="s">
+      <c r="D1" s="64"/>
+      <c r="E1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="65"/>
+      <c r="H1" s="66"/>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="66"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="27" t="s">
         <v>4</v>
       </c>
@@ -7873,7 +7857,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="G16:H65 G3:H8">
-    <cfRule type="containsText" dxfId="160" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="158" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="18">
@@ -7888,7 +7872,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66">
-    <cfRule type="containsText" dxfId="159" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="157" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H66))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -7903,7 +7887,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G15">
-    <cfRule type="containsText" dxfId="158" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="156" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G9))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -7918,7 +7902,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H15">
-    <cfRule type="containsText" dxfId="157" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="155" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H9))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="12">
@@ -7933,7 +7917,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G67:G71">
-    <cfRule type="containsText" dxfId="156" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="154" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G67))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -7948,7 +7932,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67:H71">
-    <cfRule type="containsText" dxfId="155" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="153" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H67))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -7963,7 +7947,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G66">
-    <cfRule type="containsText" dxfId="154" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="152" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G66))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7989,11 +7973,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I197"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="9" ySplit="2" topLeftCell="J153" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A123" sqref="A123:XFD123"/>
+      <selection pane="bottomRight" activeCell="J123" sqref="J123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -8007,29 +7991,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="55" t="s">
+      <c r="A1" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>341</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="62" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="65"/>
+      <c r="H1" s="66"/>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="43" t="s">
         <v>4</v>
       </c>
@@ -11655,7 +11639,7 @@
         <v>0</v>
       </c>
       <c r="H123" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I123" s="33" t="str">
         <f t="shared" si="6"/>
@@ -13885,7 +13869,7 @@
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="G4:H108 G109 G110:H167">
-    <cfRule type="containsText" dxfId="153" priority="65" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="151" priority="65" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G4))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="66">
@@ -13900,7 +13884,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G168:H168">
-    <cfRule type="containsText" dxfId="152" priority="63" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="150" priority="63" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G168))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="64">
@@ -13915,7 +13899,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G169:H169">
-    <cfRule type="containsText" dxfId="151" priority="61" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="149" priority="61" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G169))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="62">
@@ -13930,7 +13914,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G170:H170">
-    <cfRule type="containsText" dxfId="150" priority="59" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="148" priority="59" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G170))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="60">
@@ -13945,7 +13929,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G171:H171">
-    <cfRule type="containsText" dxfId="149" priority="57" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="147" priority="57" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G171))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="58">
@@ -13960,7 +13944,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G172:H172">
-    <cfRule type="containsText" dxfId="148" priority="55" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="146" priority="55" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G172))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="56">
@@ -13975,7 +13959,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G173:H173">
-    <cfRule type="containsText" dxfId="147" priority="53" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="145" priority="53" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G173))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="54">
@@ -13990,7 +13974,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G174:H174">
-    <cfRule type="containsText" dxfId="146" priority="51" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="144" priority="51" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G174))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="52">
@@ -14005,7 +13989,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G175:H175">
-    <cfRule type="containsText" dxfId="145" priority="49" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="143" priority="49" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G175))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="50">
@@ -14020,7 +14004,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G176:H176">
-    <cfRule type="containsText" dxfId="144" priority="47" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="142" priority="47" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G176))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="48">
@@ -14035,7 +14019,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G177:H177">
-    <cfRule type="containsText" dxfId="143" priority="45" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="141" priority="45" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G177))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="46">
@@ -14050,7 +14034,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G178:H178">
-    <cfRule type="containsText" dxfId="142" priority="43" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="140" priority="43" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G178))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="44">
@@ -14065,7 +14049,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G179:H179">
-    <cfRule type="containsText" dxfId="141" priority="41" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="139" priority="41" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G179))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="42">
@@ -14080,7 +14064,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G180:H180">
-    <cfRule type="containsText" dxfId="140" priority="39" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="138" priority="39" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G180))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="40">
@@ -14095,7 +14079,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G181:H181">
-    <cfRule type="containsText" dxfId="139" priority="37" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="137" priority="37" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G181))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="38">
@@ -14110,7 +14094,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G182:H182">
-    <cfRule type="containsText" dxfId="138" priority="33" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="136" priority="33" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G182))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="34">
@@ -14125,7 +14109,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G183:H183">
-    <cfRule type="containsText" dxfId="137" priority="31" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="135" priority="31" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G183))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="32">
@@ -14140,7 +14124,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G184:H184">
-    <cfRule type="containsText" dxfId="136" priority="29" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="134" priority="29" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G184))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="30">
@@ -14155,7 +14139,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G186:H186">
-    <cfRule type="containsText" dxfId="135" priority="25" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="133" priority="25" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G186))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="26">
@@ -14170,7 +14154,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G187:H187">
-    <cfRule type="containsText" dxfId="134" priority="23" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="132" priority="23" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G187))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="24">
@@ -14185,7 +14169,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188:H188">
-    <cfRule type="containsText" dxfId="133" priority="21" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="131" priority="21" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G188))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="22">
@@ -14200,7 +14184,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:H185">
-    <cfRule type="containsText" dxfId="132" priority="19" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="130" priority="19" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G185))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="20">
@@ -14215,7 +14199,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G189:H189">
-    <cfRule type="containsText" dxfId="131" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="129" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G189))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="18">
@@ -14230,7 +14214,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G190:H190">
-    <cfRule type="containsText" dxfId="130" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="128" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G190))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -14245,7 +14229,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:H191">
-    <cfRule type="containsText" dxfId="129" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="127" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G191))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -14260,7 +14244,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109">
-    <cfRule type="containsText" dxfId="128" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="126" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H109))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14277,7 +14261,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:H3">
-    <cfRule type="containsText" dxfId="127" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="125" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -14292,7 +14276,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G192">
-    <cfRule type="containsText" dxfId="126" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="124" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G192))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -14307,7 +14291,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H192">
-    <cfRule type="containsText" dxfId="125" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="123" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H192))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -14322,7 +14306,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G193:H193 G195:H195 G197:H197">
-    <cfRule type="containsText" dxfId="124" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="122" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G193))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -14337,7 +14321,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G194:H194 G196:H196">
-    <cfRule type="containsText" dxfId="123" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="121" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G194))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -14361,8 +14345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="9" ySplit="2" topLeftCell="J45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
@@ -14379,29 +14363,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="55" t="s">
+      <c r="A1" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>341</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="62" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="65" t="s">
         <v>306</v>
       </c>
-      <c r="H1" s="65"/>
+      <c r="H1" s="66"/>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="27" t="s">
         <v>4</v>
       </c>
@@ -15220,7 +15204,7 @@
       <c r="F30" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="G30" s="67">
+      <c r="G30" s="53">
         <v>1</v>
       </c>
       <c r="H30" s="12" t="s">
@@ -16881,7 +16865,7 @@
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="G15:H15 G17:H17 G26:H26 G19:H20 G22:H24">
-    <cfRule type="containsText" dxfId="122" priority="366" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="120" priority="366" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G15))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="367">
@@ -16896,7 +16880,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="containsText" dxfId="121" priority="347" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="119" priority="347" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H26))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16913,7 +16897,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:H28">
-    <cfRule type="containsText" dxfId="120" priority="345" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="118" priority="345" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G28))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="346">
@@ -16928,7 +16912,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="containsText" dxfId="119" priority="343" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="117" priority="343" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H28))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16945,7 +16929,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30:H30">
-    <cfRule type="containsText" dxfId="118" priority="341" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="116" priority="341" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G30))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="342">
@@ -16960,7 +16944,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsText" dxfId="117" priority="339" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="115" priority="339" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H30))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16977,7 +16961,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:H32">
-    <cfRule type="containsText" dxfId="116" priority="333" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="114" priority="333" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G32))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="334">
@@ -16992,7 +16976,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="containsText" dxfId="115" priority="331" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="113" priority="331" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H32))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17009,7 +16993,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:H34 G38:H38">
-    <cfRule type="containsText" dxfId="114" priority="329" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="112" priority="329" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G34))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="330">
@@ -17024,11 +17008,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34 H38">
-    <cfRule type="containsText" dxfId="113" priority="327" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="111" priority="327" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H34))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H38 H34">
+  <conditionalFormatting sqref="H34 H38">
     <cfRule type="colorScale" priority="328">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17041,7 +17025,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33:H33 G36:H36 G40:H40">
-    <cfRule type="containsText" dxfId="112" priority="325" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="110" priority="325" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G33))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="326">
@@ -17056,11 +17040,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33 H36 H40">
-    <cfRule type="containsText" dxfId="111" priority="323" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="109" priority="323" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H33))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36 H33 H40">
+  <conditionalFormatting sqref="H33 H36 H40">
     <cfRule type="colorScale" priority="324">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17073,7 +17057,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:H42">
-    <cfRule type="containsText" dxfId="110" priority="321" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="108" priority="321" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G42))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="322">
@@ -17088,7 +17072,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="containsText" dxfId="109" priority="319" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="107" priority="319" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H42))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17105,7 +17089,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:H43">
-    <cfRule type="containsText" dxfId="108" priority="317" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="106" priority="317" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G43))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="318">
@@ -17120,7 +17104,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="containsText" dxfId="107" priority="315" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="105" priority="315" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H43))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17137,7 +17121,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:H45">
-    <cfRule type="containsText" dxfId="106" priority="313" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="104" priority="313" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G45))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="314">
@@ -17152,7 +17136,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="containsText" dxfId="105" priority="311" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="103" priority="311" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H45))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17169,7 +17153,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47:H47 G49:H49 G51:H51 G53:H53 G55:H56 G54">
-    <cfRule type="containsText" dxfId="104" priority="309" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="102" priority="309" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G47))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="310">
@@ -17184,11 +17168,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47 H49 H51 H53 H55:H56">
-    <cfRule type="containsText" dxfId="103" priority="307" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="101" priority="307" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H47))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H49 H47 H51 H53 H55:H56">
+  <conditionalFormatting sqref="H47 H49 H51 H53 H55:H56">
     <cfRule type="colorScale" priority="308">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17201,7 +17185,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48:H48 G50:H50 G52:H52 H54">
-    <cfRule type="containsText" dxfId="102" priority="305" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="100" priority="305" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G48))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="306">
@@ -17216,11 +17200,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48 H50 H52 H54">
-    <cfRule type="containsText" dxfId="101" priority="303" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="99" priority="303" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H48))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50 H48 H52 H54">
+  <conditionalFormatting sqref="H48 H50 H52 H54">
     <cfRule type="colorScale" priority="304">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17233,7 +17217,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G61:H61 G63:H63 G65:H65 G67:H67 G69:H69">
-    <cfRule type="containsText" dxfId="100" priority="281" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="98" priority="281" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G61))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="282">
@@ -17248,11 +17232,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61 H63 H65 H67 H69">
-    <cfRule type="containsText" dxfId="99" priority="279" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="97" priority="279" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H61))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63 H61 H65 H67 H69">
+  <conditionalFormatting sqref="H61 H63 H65 H67 H69">
     <cfRule type="colorScale" priority="280">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17265,7 +17249,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60:H60 G62:H62 G64:H64 G66:H66 G68:H68 G70:H70 G73:H73">
-    <cfRule type="containsText" dxfId="98" priority="277" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="96" priority="277" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G60))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="278">
@@ -17280,11 +17264,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60 H62 H64 H66 H68 H70 H73">
-    <cfRule type="containsText" dxfId="97" priority="275" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="95" priority="275" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H60))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H62 H60 H64 H66 H68 H70 H73">
+  <conditionalFormatting sqref="H60 H62 H64 H66 H68 H70 H73">
     <cfRule type="colorScale" priority="276">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -17297,7 +17281,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G58:H58">
-    <cfRule type="containsText" dxfId="96" priority="273" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="94" priority="273" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G58))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="274">
@@ -17312,7 +17296,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="containsText" dxfId="95" priority="271" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="93" priority="271" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H58))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17329,7 +17313,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G71:H71">
-    <cfRule type="containsText" dxfId="94" priority="269" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="92" priority="269" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G71))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="270">
@@ -17344,7 +17328,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71">
-    <cfRule type="containsText" dxfId="93" priority="267" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="91" priority="267" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H71))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17361,7 +17345,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="containsText" dxfId="92" priority="253" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="90" priority="253" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G22))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="254">
@@ -17376,7 +17360,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="91" priority="251" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="89" priority="251" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H22))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="252">
@@ -17391,7 +17375,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="containsText" dxfId="90" priority="249" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="88" priority="249" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G25))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="250">
@@ -17406,7 +17390,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27:H27">
-    <cfRule type="containsText" dxfId="89" priority="241" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="87" priority="241" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G27))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="242">
@@ -17421,7 +17405,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="containsText" dxfId="88" priority="239" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="86" priority="239" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H27))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17438,7 +17422,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G75:H75">
-    <cfRule type="containsText" dxfId="87" priority="189" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="85" priority="189" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G75))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="190">
@@ -17453,7 +17437,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="containsText" dxfId="86" priority="187" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="84" priority="187" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H75))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17470,7 +17454,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G77:H77">
-    <cfRule type="containsText" dxfId="85" priority="181" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="83" priority="181" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G77))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="182">
@@ -17485,7 +17469,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="containsText" dxfId="84" priority="179" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="82" priority="179" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H77))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17502,7 +17486,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:H79">
-    <cfRule type="containsText" dxfId="83" priority="173" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="81" priority="173" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G79))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="174">
@@ -17517,7 +17501,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="containsText" dxfId="82" priority="171" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="80" priority="171" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H79))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17534,7 +17518,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81:H81">
-    <cfRule type="containsText" dxfId="81" priority="169" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="79" priority="169" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G81))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="170">
@@ -17549,7 +17533,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81">
-    <cfRule type="containsText" dxfId="80" priority="167" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="78" priority="167" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H81))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17566,7 +17550,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83:H83">
-    <cfRule type="containsText" dxfId="79" priority="165" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="77" priority="165" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G83))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="166">
@@ -17581,7 +17565,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="containsText" dxfId="78" priority="163" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="76" priority="163" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H83))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17598,7 +17582,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G85:H85">
-    <cfRule type="containsText" dxfId="77" priority="161" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="75" priority="161" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G85))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="162">
@@ -17613,7 +17597,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="containsText" dxfId="76" priority="159" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="74" priority="159" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H85))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17630,7 +17614,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G27">
-    <cfRule type="containsText" dxfId="75" priority="141" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="73" priority="141" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G27))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17647,7 +17631,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:H29">
-    <cfRule type="containsText" dxfId="74" priority="139" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="72" priority="139" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G29))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="140">
@@ -17662,7 +17646,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="containsText" dxfId="73" priority="137" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="71" priority="137" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H29))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17679,7 +17663,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="containsText" dxfId="72" priority="135" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="70" priority="135" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G29))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17696,7 +17680,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35:H35">
-    <cfRule type="containsText" dxfId="71" priority="133" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="69" priority="133" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G35))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="134">
@@ -17711,7 +17695,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="containsText" dxfId="70" priority="131" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="68" priority="131" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H35))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17728,7 +17712,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="69" priority="129" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="67" priority="129" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G35))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17745,7 +17729,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44:H44">
-    <cfRule type="containsText" dxfId="68" priority="127" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="66" priority="127" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G44))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="128">
@@ -17760,7 +17744,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="containsText" dxfId="67" priority="125" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="65" priority="125" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H44))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17777,7 +17761,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44">
-    <cfRule type="containsText" dxfId="66" priority="123" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="64" priority="123" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G44))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17794,7 +17778,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46:H46">
-    <cfRule type="containsText" dxfId="65" priority="121" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="63" priority="121" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G46))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="122">
@@ -17809,7 +17793,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="containsText" dxfId="64" priority="119" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="62" priority="119" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H46))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17826,7 +17810,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46">
-    <cfRule type="containsText" dxfId="63" priority="117" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="61" priority="117" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G46))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17843,7 +17827,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G59:H59">
-    <cfRule type="containsText" dxfId="62" priority="115" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="60" priority="115" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G59))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="116">
@@ -17858,7 +17842,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="containsText" dxfId="61" priority="113" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="59" priority="113" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H59))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17875,7 +17859,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G59">
-    <cfRule type="containsText" dxfId="60" priority="111" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="58" priority="111" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G59))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17892,7 +17876,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:H57">
-    <cfRule type="containsText" dxfId="59" priority="109" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="57" priority="109" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G57))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="110">
@@ -17907,7 +17891,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="containsText" dxfId="58" priority="107" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="56" priority="107" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H57))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17924,7 +17908,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57">
-    <cfRule type="containsText" dxfId="57" priority="105" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="55" priority="105" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G57))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17941,7 +17925,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G80:H80">
-    <cfRule type="containsText" dxfId="56" priority="103" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="54" priority="103" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G80))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="104">
@@ -17956,7 +17940,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80">
-    <cfRule type="containsText" dxfId="55" priority="101" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="53" priority="101" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H80))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17973,7 +17957,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G80">
-    <cfRule type="containsText" dxfId="54" priority="99" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="52" priority="99" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G80))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17990,7 +17974,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G78:H78">
-    <cfRule type="containsText" dxfId="53" priority="97" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="51" priority="97" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G78))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="98">
@@ -18005,7 +17989,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78">
-    <cfRule type="containsText" dxfId="52" priority="95" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="50" priority="95" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H78))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18022,7 +18006,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G78">
-    <cfRule type="containsText" dxfId="51" priority="93" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="49" priority="93" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G78))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18039,7 +18023,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76:H76">
-    <cfRule type="containsText" dxfId="50" priority="91" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="48" priority="91" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G76))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="92">
@@ -18054,7 +18038,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76">
-    <cfRule type="containsText" dxfId="49" priority="89" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="47" priority="89" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H76))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18071,7 +18055,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76">
-    <cfRule type="containsText" dxfId="48" priority="87" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="46" priority="87" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G76))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18088,7 +18072,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G74:H74">
-    <cfRule type="containsText" dxfId="47" priority="85" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="45" priority="85" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G74))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="86">
@@ -18103,7 +18087,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74">
-    <cfRule type="containsText" dxfId="46" priority="83" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="44" priority="83" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H74))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18120,7 +18104,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G74">
-    <cfRule type="containsText" dxfId="45" priority="81" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="43" priority="81" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G74))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18137,7 +18121,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G72:H72">
-    <cfRule type="containsText" dxfId="44" priority="79" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="42" priority="79" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G72))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="80">
@@ -18152,7 +18136,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72">
-    <cfRule type="containsText" dxfId="43" priority="77" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="41" priority="77" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H72))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18169,7 +18153,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G72">
-    <cfRule type="containsText" dxfId="42" priority="75" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="40" priority="75" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G72))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18186,7 +18170,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82:H82">
-    <cfRule type="containsText" dxfId="41" priority="73" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="39" priority="73" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G82))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="74">
@@ -18201,7 +18185,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="containsText" dxfId="40" priority="71" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="38" priority="71" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H82))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18218,7 +18202,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82">
-    <cfRule type="containsText" dxfId="39" priority="69" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="37" priority="69" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G82))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18235,7 +18219,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86:H86">
-    <cfRule type="containsText" dxfId="38" priority="67" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="36" priority="67" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G86))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="68">
@@ -18250,7 +18234,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="containsText" dxfId="37" priority="65" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="35" priority="65" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H86))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18267,7 +18251,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G86">
-    <cfRule type="containsText" dxfId="36" priority="63" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="34" priority="63" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G86))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18284,7 +18268,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G84:H84">
-    <cfRule type="containsText" dxfId="35" priority="61" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="33" priority="61" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G84))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="62">
@@ -18299,7 +18283,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="containsText" dxfId="34" priority="59" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="32" priority="59" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H84))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18316,7 +18300,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G84">
-    <cfRule type="containsText" dxfId="33" priority="57" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="31" priority="57" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G84))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18333,7 +18317,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:H37">
-    <cfRule type="containsText" dxfId="32" priority="55" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="30" priority="55" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G37))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="56">
@@ -18348,7 +18332,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="containsText" dxfId="31" priority="53" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="29" priority="53" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H37))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18365,7 +18349,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="containsText" dxfId="30" priority="51" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="28" priority="51" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G37))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18382,7 +18366,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41:H41">
-    <cfRule type="containsText" dxfId="29" priority="49" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="27" priority="49" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G41))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="50">
@@ -18397,7 +18381,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="containsText" dxfId="28" priority="47" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="26" priority="47" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H41))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18414,7 +18398,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41">
-    <cfRule type="containsText" dxfId="27" priority="45" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="25" priority="45" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G41))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18431,7 +18415,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39:H39">
-    <cfRule type="containsText" dxfId="26" priority="43" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="24" priority="43" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G39))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="44">
@@ -18446,7 +18430,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="containsText" dxfId="25" priority="41" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="23" priority="41" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H39))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18463,7 +18447,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="containsText" dxfId="24" priority="39" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="22" priority="39" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G39))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18480,7 +18464,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="containsText" dxfId="23" priority="37" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="21" priority="37" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H25))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="38">
@@ -18495,7 +18479,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="containsText" dxfId="22" priority="35" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="20" priority="35" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G21))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="36">
@@ -18510,7 +18494,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="21" priority="33" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="19" priority="33" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H21))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="34">
@@ -18525,7 +18509,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="18" priority="31" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G18))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="32">
@@ -18540,7 +18524,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="17" priority="29" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H18))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="30">
@@ -18555,7 +18539,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="containsText" dxfId="18" priority="27" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="16" priority="27" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G16))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="28">
@@ -18570,7 +18554,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="26">
@@ -18585,7 +18569,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G30))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18602,7 +18586,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:H31">
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G31))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="22">
@@ -18617,7 +18601,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="12" priority="19" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H31))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18634,7 +18618,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G31))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18651,7 +18635,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:H8">
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -18666,7 +18650,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G14">
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G9))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -18681,7 +18665,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H14">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H9))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="12">
@@ -18696,7 +18680,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G87:H87">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G87))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -18711,7 +18695,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H87))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18728,7 +18712,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88:H88">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G88))))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -18743,7 +18727,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H88))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18760,7 +18744,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G88))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>